<commit_message>
Burn Chart, amended planned formula
</commit_message>
<xml_diff>
--- a/Burn Chart.xlsx
+++ b/Burn Chart.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/fa997cf651389d1a/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DavidPortas\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="51" documentId="8_{806BCFEB-728E-4239-B065-50286AB97B21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{B3E4AB2D-CAA5-46D2-A7B5-23DFA56AD685}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{538F88C7-AC5F-4676-B361-7B10FE2C8DC9}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3720" yWindow="2010" windowWidth="22800" windowHeight="13485" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Burn Chart" sheetId="3" r:id="rId1"/>
@@ -673,32 +673,8 @@
     <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="18" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="22" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -712,43 +688,67 @@
     <xf numFmtId="0" fontId="23" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="24" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -936,37 +936,37 @@
                   <c:v>1300</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1300</c:v>
+                  <c:v>1350</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1082,31 +1082,31 @@
                   <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>290</c:v>
+                  <c:v>210</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>400</c:v>
+                  <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>510</c:v>
+                  <c:v>405</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>610</c:v>
+                  <c:v>515</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>730</c:v>
+                  <c:v>645</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>850</c:v>
+                  <c:v>775</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>990</c:v>
+                  <c:v>940</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1130</c:v>
+                  <c:v>1095</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1270</c:v>
+                  <c:v>1265</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1244,25 +1244,25 @@
                   <c:v>295</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>390</c:v>
+                  <c:v>415</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>490</c:v>
+                  <c:v>525</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>610</c:v>
+                  <c:v>655</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>730</c:v>
+                  <c:v>800</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>860</c:v>
+                  <c:v>955</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1000</c:v>
+                  <c:v>1125</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1135</c:v>
+                  <c:v>1285</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1601,6 +1601,239 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>4</xdr:row>
+      <xdr:rowOff>9524</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{DA8ED4BA-242E-4812-AF4C-488D03412024}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="4076700" y="628649"/>
+          <a:ext cx="361950" cy="438151"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" lIns="0" tIns="0" rIns="0" bIns="0" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Story</a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100" baseline="0"/>
+            <a:t>Points</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-GB" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>23</xdr:row>
+      <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>501865</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>77220</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="TextBox 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5B009982-9CC5-4D32-AE1E-1C201D68168D}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="8867775" y="4276725"/>
+          <a:ext cx="644740" cy="229620"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:txBody>
+        <a:bodyPr wrap="square" rtlCol="0"/>
+        <a:lstStyle>
+          <a:lvl1pPr marL="0" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl1pPr>
+          <a:lvl2pPr marL="457200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl2pPr>
+          <a:lvl3pPr marL="914400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl3pPr>
+          <a:lvl4pPr marL="1371600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl4pPr>
+          <a:lvl5pPr marL="1828800" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl5pPr>
+          <a:lvl6pPr marL="2286000" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl6pPr>
+          <a:lvl7pPr marL="2743200" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl7pPr>
+          <a:lvl8pPr marL="3200400" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl8pPr>
+          <a:lvl9pPr marL="3657600" indent="0">
+            <a:defRPr sz="1100">
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:lvl9pPr>
+        </a:lstStyle>
+        <a:p>
+          <a:pPr algn="r"/>
+          <a:r>
+            <a:rPr lang="en-GB" sz="1100"/>
+            <a:t>Sprints</a:t>
+          </a:r>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -1931,7 +2164,7 @@
   <dimension ref="A2:U30"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B28" sqref="B28"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1947,67 +2180,67 @@
   <sheetData>
     <row r="2" spans="1:21" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="4"/>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="12"/>
-      <c r="D2" s="12"/>
-      <c r="E2" s="12"/>
-      <c r="F2" s="12"/>
-      <c r="G2" s="12"/>
+      <c r="C2" s="38"/>
+      <c r="D2" s="38"/>
+      <c r="E2" s="38"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
       <c r="H2" s="4"/>
-      <c r="I2" s="18" t="s">
+      <c r="I2" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="J2" s="19"/>
-      <c r="K2" s="19"/>
-      <c r="L2" s="19"/>
-      <c r="M2" s="19"/>
-      <c r="N2" s="19"/>
-      <c r="O2" s="19"/>
-      <c r="P2" s="19"/>
-      <c r="Q2" s="19"/>
-      <c r="R2" s="19"/>
+      <c r="J2" s="36"/>
+      <c r="K2" s="36"/>
+      <c r="L2" s="36"/>
+      <c r="M2" s="36"/>
+      <c r="N2" s="36"/>
+      <c r="O2" s="36"/>
+      <c r="P2" s="36"/>
+      <c r="Q2" s="36"/>
+      <c r="R2" s="36"/>
       <c r="S2" s="4"/>
       <c r="T2" s="10" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="3" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="20"/>
-      <c r="B3" s="23"/>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23"/>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23"/>
-      <c r="G3" s="23"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="21"/>
-      <c r="J3" s="21"/>
-      <c r="K3" s="21"/>
-      <c r="L3" s="21"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="21"/>
-      <c r="O3" s="21"/>
-      <c r="P3" s="21"/>
-      <c r="Q3" s="21"/>
-      <c r="R3" s="21"/>
-      <c r="S3" s="21"/>
-      <c r="T3" s="25"/>
-      <c r="U3" s="22"/>
+      <c r="A3" s="12"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="15"/>
+      <c r="D3" s="15"/>
+      <c r="E3" s="15"/>
+      <c r="F3" s="15"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="13"/>
+      <c r="I3" s="13"/>
+      <c r="J3" s="13"/>
+      <c r="K3" s="13"/>
+      <c r="L3" s="13"/>
+      <c r="M3" s="13"/>
+      <c r="N3" s="13"/>
+      <c r="O3" s="13"/>
+      <c r="P3" s="13"/>
+      <c r="Q3" s="13"/>
+      <c r="R3" s="13"/>
+      <c r="S3" s="13"/>
+      <c r="T3" s="17"/>
+      <c r="U3" s="14"/>
     </row>
     <row r="4" spans="1:21" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="13" t="s">
+      <c r="B4" s="16"/>
+      <c r="C4" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="D4" s="14"/>
-      <c r="E4" s="13" t="s">
+      <c r="D4" s="32"/>
+      <c r="E4" s="31" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="14"/>
-      <c r="G4" s="15" t="s">
+      <c r="F4" s="32"/>
+      <c r="G4" s="33" t="s">
         <v>4</v>
       </c>
       <c r="H4" s="4"/>
@@ -2022,14 +2255,14 @@
       <c r="Q4" s="4"/>
       <c r="R4" s="4"/>
       <c r="S4" s="4"/>
-      <c r="T4" s="26">
+      <c r="T4" s="29">
         <f>D15</f>
-        <v>135</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="11" t="s">
         <v>5</v>
       </c>
       <c r="C5" s="8" t="s">
@@ -2044,7 +2277,7 @@
       <c r="F5" s="9" t="s">
         <v>1</v>
       </c>
-      <c r="G5" s="16"/>
+      <c r="G5" s="34"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
       <c r="J5" s="4"/>
@@ -2057,28 +2290,28 @@
       <c r="Q5" s="4"/>
       <c r="R5" s="4"/>
       <c r="S5" s="4"/>
-      <c r="T5" s="27"/>
+      <c r="T5" s="30"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A6" s="6"/>
-      <c r="B6" s="30">
+      <c r="B6" s="20">
         <v>1</v>
       </c>
-      <c r="C6" s="31">
+      <c r="C6" s="21">
         <v>160</v>
       </c>
-      <c r="D6" s="31">
+      <c r="D6" s="21">
         <v>80</v>
       </c>
-      <c r="E6" s="32">
+      <c r="E6" s="22">
         <f>C6</f>
         <v>160</v>
       </c>
-      <c r="F6" s="32">
+      <c r="F6" s="22">
         <f>D6</f>
         <v>80</v>
       </c>
-      <c r="G6" s="33">
+      <c r="G6" s="23">
         <v>170</v>
       </c>
       <c r="H6" s="4"/>
@@ -2096,25 +2329,25 @@
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A7" s="6"/>
-      <c r="B7" s="34">
+      <c r="B7" s="24">
         <f>B6+1</f>
         <v>2</v>
       </c>
-      <c r="C7" s="31">
+      <c r="C7" s="21">
         <v>130</v>
       </c>
-      <c r="D7" s="31">
+      <c r="D7" s="21">
         <v>105</v>
       </c>
-      <c r="E7" s="32">
-        <f t="shared" ref="E7:E15" si="0">E6+C7</f>
-        <v>290</v>
-      </c>
-      <c r="F7" s="32">
-        <f t="shared" ref="F7:F15" si="1">F6+D7</f>
+      <c r="E7" s="22">
+        <f>F6+C7</f>
+        <v>210</v>
+      </c>
+      <c r="F7" s="22">
+        <f t="shared" ref="F7:F15" si="0">F6+D7</f>
         <v>185</v>
       </c>
-      <c r="G7" s="33">
+      <c r="G7" s="23">
         <v>300</v>
       </c>
       <c r="H7" s="4"/>
@@ -2132,25 +2365,25 @@
     </row>
     <row r="8" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A8" s="6"/>
-      <c r="B8" s="34">
-        <f t="shared" ref="B8:B24" si="2">B7+1</f>
+      <c r="B8" s="24">
+        <f t="shared" ref="B8:B24" si="1">B7+1</f>
         <v>3</v>
       </c>
-      <c r="C8" s="31">
+      <c r="C8" s="21">
         <v>110</v>
       </c>
-      <c r="D8" s="31">
+      <c r="D8" s="21">
         <v>110</v>
       </c>
-      <c r="E8" s="32">
+      <c r="E8" s="22">
+        <f t="shared" ref="E8:E15" si="2">F7+C8</f>
+        <v>295</v>
+      </c>
+      <c r="F8" s="22">
         <f t="shared" si="0"/>
-        <v>400</v>
-      </c>
-      <c r="F8" s="32">
-        <f t="shared" si="1"/>
         <v>295</v>
       </c>
-      <c r="G8" s="33">
+      <c r="G8" s="23">
         <v>400</v>
       </c>
       <c r="H8" s="4"/>
@@ -2168,25 +2401,25 @@
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A9" s="6"/>
-      <c r="B9" s="34">
+      <c r="B9" s="24">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="C9" s="21">
+        <v>110</v>
+      </c>
+      <c r="D9" s="21">
+        <v>120</v>
+      </c>
+      <c r="E9" s="22">
         <f t="shared" si="2"/>
-        <v>4</v>
-      </c>
-      <c r="C9" s="31">
-        <v>110</v>
-      </c>
-      <c r="D9" s="31">
-        <v>95</v>
-      </c>
-      <c r="E9" s="32">
+        <v>405</v>
+      </c>
+      <c r="F9" s="22">
         <f t="shared" si="0"/>
-        <v>510</v>
-      </c>
-      <c r="F9" s="32">
-        <f t="shared" si="1"/>
-        <v>390</v>
-      </c>
-      <c r="G9" s="33">
+        <v>415</v>
+      </c>
+      <c r="G9" s="23">
         <v>510</v>
       </c>
       <c r="H9" s="4"/>
@@ -2204,25 +2437,25 @@
     </row>
     <row r="10" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A10" s="6"/>
-      <c r="B10" s="34">
+      <c r="B10" s="24">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="C10" s="21">
+        <v>100</v>
+      </c>
+      <c r="D10" s="21">
+        <v>110</v>
+      </c>
+      <c r="E10" s="22">
         <f t="shared" si="2"/>
-        <v>5</v>
-      </c>
-      <c r="C10" s="31">
-        <v>100</v>
-      </c>
-      <c r="D10" s="31">
-        <v>100</v>
-      </c>
-      <c r="E10" s="32">
+        <v>515</v>
+      </c>
+      <c r="F10" s="22">
         <f t="shared" si="0"/>
-        <v>610</v>
-      </c>
-      <c r="F10" s="32">
-        <f t="shared" si="1"/>
-        <v>490</v>
-      </c>
-      <c r="G10" s="33">
+        <v>525</v>
+      </c>
+      <c r="G10" s="23">
         <v>700</v>
       </c>
       <c r="H10" s="4"/>
@@ -2240,25 +2473,25 @@
     </row>
     <row r="11" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A11" s="6"/>
-      <c r="B11" s="34">
+      <c r="B11" s="24">
+        <f t="shared" si="1"/>
+        <v>6</v>
+      </c>
+      <c r="C11" s="21">
+        <v>120</v>
+      </c>
+      <c r="D11" s="21">
+        <v>130</v>
+      </c>
+      <c r="E11" s="22">
         <f t="shared" si="2"/>
-        <v>6</v>
-      </c>
-      <c r="C11" s="31">
-        <v>120</v>
-      </c>
-      <c r="D11" s="31">
-        <v>120</v>
-      </c>
-      <c r="E11" s="32">
+        <v>645</v>
+      </c>
+      <c r="F11" s="22">
         <f t="shared" si="0"/>
-        <v>730</v>
-      </c>
-      <c r="F11" s="32">
-        <f t="shared" si="1"/>
-        <v>610</v>
-      </c>
-      <c r="G11" s="33">
+        <v>655</v>
+      </c>
+      <c r="G11" s="23">
         <v>990</v>
       </c>
       <c r="H11" s="4"/>
@@ -2276,25 +2509,25 @@
     </row>
     <row r="12" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A12" s="6"/>
-      <c r="B12" s="34">
+      <c r="B12" s="24">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
+      <c r="C12" s="21">
+        <v>120</v>
+      </c>
+      <c r="D12" s="21">
+        <v>145</v>
+      </c>
+      <c r="E12" s="22">
         <f t="shared" si="2"/>
-        <v>7</v>
-      </c>
-      <c r="C12" s="31">
-        <v>120</v>
-      </c>
-      <c r="D12" s="31">
-        <v>120</v>
-      </c>
-      <c r="E12" s="32">
+        <v>775</v>
+      </c>
+      <c r="F12" s="22">
         <f t="shared" si="0"/>
-        <v>850</v>
-      </c>
-      <c r="F12" s="32">
-        <f t="shared" si="1"/>
-        <v>730</v>
-      </c>
-      <c r="G12" s="33">
+        <v>800</v>
+      </c>
+      <c r="G12" s="23">
         <v>1000</v>
       </c>
       <c r="H12" s="4"/>
@@ -2312,25 +2545,25 @@
     </row>
     <row r="13" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A13" s="6"/>
-      <c r="B13" s="34">
+      <c r="B13" s="24">
+        <f t="shared" si="1"/>
+        <v>8</v>
+      </c>
+      <c r="C13" s="21">
+        <v>140</v>
+      </c>
+      <c r="D13" s="21">
+        <v>155</v>
+      </c>
+      <c r="E13" s="22">
         <f t="shared" si="2"/>
-        <v>8</v>
-      </c>
-      <c r="C13" s="31">
-        <v>140</v>
-      </c>
-      <c r="D13" s="31">
-        <v>130</v>
-      </c>
-      <c r="E13" s="32">
+        <v>940</v>
+      </c>
+      <c r="F13" s="22">
         <f t="shared" si="0"/>
-        <v>990</v>
-      </c>
-      <c r="F13" s="32">
-        <f t="shared" si="1"/>
-        <v>860</v>
-      </c>
-      <c r="G13" s="33">
+        <v>955</v>
+      </c>
+      <c r="G13" s="23">
         <v>1200</v>
       </c>
       <c r="H13" s="4"/>
@@ -2348,25 +2581,25 @@
     </row>
     <row r="14" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A14" s="6"/>
-      <c r="B14" s="34">
+      <c r="B14" s="24">
+        <f t="shared" si="1"/>
+        <v>9</v>
+      </c>
+      <c r="C14" s="21">
+        <v>140</v>
+      </c>
+      <c r="D14" s="21">
+        <v>170</v>
+      </c>
+      <c r="E14" s="22">
         <f t="shared" si="2"/>
-        <v>9</v>
-      </c>
-      <c r="C14" s="31">
-        <v>140</v>
-      </c>
-      <c r="D14" s="31">
-        <v>140</v>
-      </c>
-      <c r="E14" s="32">
+        <v>1095</v>
+      </c>
+      <c r="F14" s="22">
         <f t="shared" si="0"/>
-        <v>1130</v>
-      </c>
-      <c r="F14" s="32">
-        <f t="shared" si="1"/>
-        <v>1000</v>
-      </c>
-      <c r="G14" s="33">
+        <v>1125</v>
+      </c>
+      <c r="G14" s="23">
         <v>1300</v>
       </c>
       <c r="H14" s="4"/>
@@ -2384,26 +2617,26 @@
     </row>
     <row r="15" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A15" s="6"/>
-      <c r="B15" s="34">
+      <c r="B15" s="24">
+        <f t="shared" si="1"/>
+        <v>10</v>
+      </c>
+      <c r="C15" s="21">
+        <v>140</v>
+      </c>
+      <c r="D15" s="21">
+        <v>160</v>
+      </c>
+      <c r="E15" s="22">
         <f t="shared" si="2"/>
-        <v>10</v>
-      </c>
-      <c r="C15" s="31">
-        <v>140</v>
-      </c>
-      <c r="D15" s="31">
-        <v>135</v>
-      </c>
-      <c r="E15" s="32">
+        <v>1265</v>
+      </c>
+      <c r="F15" s="22">
         <f t="shared" si="0"/>
-        <v>1270</v>
-      </c>
-      <c r="F15" s="32">
-        <f t="shared" si="1"/>
-        <v>1135</v>
-      </c>
-      <c r="G15" s="33">
-        <v>1300</v>
+        <v>1285</v>
+      </c>
+      <c r="G15" s="23">
+        <v>1350</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4"/>
@@ -2420,16 +2653,16 @@
     </row>
     <row r="16" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A16" s="6"/>
-      <c r="B16" s="34">
-        <f t="shared" si="2"/>
+      <c r="B16" s="24">
+        <f t="shared" si="1"/>
         <v>11</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
-      <c r="F16" s="32"/>
-      <c r="G16" s="33">
-        <v>1300</v>
+      <c r="C16" s="21"/>
+      <c r="D16" s="21"/>
+      <c r="E16" s="22"/>
+      <c r="F16" s="22"/>
+      <c r="G16" s="23">
+        <v>1350</v>
       </c>
       <c r="H16" s="4"/>
       <c r="I16" s="4"/>
@@ -2446,16 +2679,16 @@
     </row>
     <row r="17" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A17" s="6"/>
-      <c r="B17" s="34">
-        <f t="shared" si="2"/>
+      <c r="B17" s="24">
+        <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="C17" s="31"/>
-      <c r="D17" s="31"/>
-      <c r="E17" s="32"/>
-      <c r="F17" s="32"/>
-      <c r="G17" s="33">
-        <v>1300</v>
+      <c r="C17" s="21"/>
+      <c r="D17" s="21"/>
+      <c r="E17" s="22"/>
+      <c r="F17" s="22"/>
+      <c r="G17" s="23">
+        <v>1350</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4"/>
@@ -2472,16 +2705,16 @@
     </row>
     <row r="18" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A18" s="6"/>
-      <c r="B18" s="34">
-        <f t="shared" si="2"/>
+      <c r="B18" s="24">
+        <f t="shared" si="1"/>
         <v>13</v>
       </c>
-      <c r="C18" s="31"/>
-      <c r="D18" s="31"/>
-      <c r="E18" s="32"/>
-      <c r="F18" s="32"/>
-      <c r="G18" s="33">
-        <v>1300</v>
+      <c r="C18" s="21"/>
+      <c r="D18" s="21"/>
+      <c r="E18" s="22"/>
+      <c r="F18" s="22"/>
+      <c r="G18" s="23">
+        <v>1350</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4"/>
@@ -2498,16 +2731,16 @@
     </row>
     <row r="19" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A19" s="6"/>
-      <c r="B19" s="34">
-        <f t="shared" si="2"/>
+      <c r="B19" s="24">
+        <f t="shared" si="1"/>
         <v>14</v>
       </c>
-      <c r="C19" s="31"/>
-      <c r="D19" s="31"/>
-      <c r="E19" s="32"/>
-      <c r="F19" s="32"/>
-      <c r="G19" s="33">
-        <v>1300</v>
+      <c r="C19" s="21"/>
+      <c r="D19" s="21"/>
+      <c r="E19" s="22"/>
+      <c r="F19" s="22"/>
+      <c r="G19" s="23">
+        <v>1350</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4"/>
@@ -2524,16 +2757,16 @@
     </row>
     <row r="20" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A20" s="6"/>
-      <c r="B20" s="34">
-        <f t="shared" si="2"/>
+      <c r="B20" s="24">
+        <f t="shared" si="1"/>
         <v>15</v>
       </c>
-      <c r="C20" s="31"/>
-      <c r="D20" s="31"/>
-      <c r="E20" s="32"/>
-      <c r="F20" s="32"/>
-      <c r="G20" s="33">
-        <v>1300</v>
+      <c r="C20" s="21"/>
+      <c r="D20" s="21"/>
+      <c r="E20" s="22"/>
+      <c r="F20" s="22"/>
+      <c r="G20" s="23">
+        <v>1350</v>
       </c>
       <c r="H20" s="4"/>
       <c r="I20" s="4"/>
@@ -2550,16 +2783,16 @@
     </row>
     <row r="21" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A21" s="6"/>
-      <c r="B21" s="34">
-        <f t="shared" si="2"/>
+      <c r="B21" s="24">
+        <f t="shared" si="1"/>
         <v>16</v>
       </c>
-      <c r="C21" s="31"/>
-      <c r="D21" s="31"/>
-      <c r="E21" s="32"/>
-      <c r="F21" s="32"/>
-      <c r="G21" s="33">
-        <v>1300</v>
+      <c r="C21" s="21"/>
+      <c r="D21" s="21"/>
+      <c r="E21" s="22"/>
+      <c r="F21" s="22"/>
+      <c r="G21" s="23">
+        <v>1350</v>
       </c>
       <c r="H21" s="4"/>
       <c r="I21" s="4"/>
@@ -2576,16 +2809,16 @@
     </row>
     <row r="22" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A22" s="6"/>
-      <c r="B22" s="34">
-        <f t="shared" si="2"/>
+      <c r="B22" s="24">
+        <f t="shared" si="1"/>
         <v>17</v>
       </c>
-      <c r="C22" s="31"/>
-      <c r="D22" s="31"/>
-      <c r="E22" s="32"/>
-      <c r="F22" s="32"/>
-      <c r="G22" s="33">
-        <v>1300</v>
+      <c r="C22" s="21"/>
+      <c r="D22" s="21"/>
+      <c r="E22" s="22"/>
+      <c r="F22" s="22"/>
+      <c r="G22" s="23">
+        <v>1350</v>
       </c>
       <c r="H22" s="4"/>
       <c r="I22" s="4"/>
@@ -2602,16 +2835,16 @@
     </row>
     <row r="23" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A23" s="6"/>
-      <c r="B23" s="34">
-        <f t="shared" si="2"/>
+      <c r="B23" s="24">
+        <f t="shared" si="1"/>
         <v>18</v>
       </c>
-      <c r="C23" s="31"/>
-      <c r="D23" s="31"/>
-      <c r="E23" s="32"/>
-      <c r="F23" s="32"/>
-      <c r="G23" s="33">
-        <v>1300</v>
+      <c r="C23" s="21"/>
+      <c r="D23" s="21"/>
+      <c r="E23" s="22"/>
+      <c r="F23" s="22"/>
+      <c r="G23" s="23">
+        <v>1350</v>
       </c>
       <c r="H23" s="4"/>
       <c r="I23" s="4"/>
@@ -2628,16 +2861,16 @@
     </row>
     <row r="24" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A24" s="6"/>
-      <c r="B24" s="34">
-        <f t="shared" si="2"/>
+      <c r="B24" s="24">
+        <f t="shared" si="1"/>
         <v>19</v>
       </c>
-      <c r="C24" s="31"/>
-      <c r="D24" s="31"/>
-      <c r="E24" s="32"/>
-      <c r="F24" s="32"/>
-      <c r="G24" s="33">
-        <v>1300</v>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="23">
+        <v>1350</v>
       </c>
       <c r="H24" s="4"/>
       <c r="I24" s="4"/>
@@ -2654,16 +2887,16 @@
     </row>
     <row r="25" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A25" s="6"/>
-      <c r="B25" s="35">
+      <c r="B25" s="25">
         <f>B24+1</f>
         <v>20</v>
       </c>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="38">
-        <v>1300</v>
+      <c r="C25" s="26"/>
+      <c r="D25" s="26"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="27"/>
+      <c r="G25" s="28">
+        <v>1350</v>
       </c>
       <c r="H25" s="4"/>
       <c r="I25" s="4"/>
@@ -2681,12 +2914,12 @@
     <row r="26" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A26" s="3"/>
       <c r="B26" s="5"/>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="D26" s="29">
+      <c r="D26" s="19">
         <f>AVERAGE(D6:D25)</f>
-        <v>113.5</v>
+        <v>128.5</v>
       </c>
       <c r="E26" s="5"/>
       <c r="F26" s="5"/>
@@ -2804,6 +3037,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100A74B1CC501571F4EA2C7167360101F8F" ma:contentTypeVersion="11" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="dcef05cbb9e0f95998c222e0a757e8c6">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="401585dc-c952-4eea-bf12-b28eb4f21e21" xmlns:ns3="ca1056d6-2406-4a1a-a945-d8b2d91a4122" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4aae57248ed27879c417f2d42eb9b1dc" ns2:_="" ns3:_="">
     <xsd:import namespace="401585dc-c952-4eea-bf12-b28eb4f21e21"/>
@@ -3014,36 +3262,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{184B6717-C458-43A8-A005-0C485A337420}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E65D5BF9-35B3-48B3-8C3D-EE8C1CB1B12C}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="401585dc-c952-4eea-bf12-b28eb4f21e21"/>
-    <ds:schemaRef ds:uri="ca1056d6-2406-4a1a-a945-d8b2d91a4122"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -3066,9 +3288,20 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E65D5BF9-35B3-48B3-8C3D-EE8C1CB1B12C}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{184B6717-C458-43A8-A005-0C485A337420}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="401585dc-c952-4eea-bf12-b28eb4f21e21"/>
+    <ds:schemaRef ds:uri="ca1056d6-2406-4a1a-a945-d8b2d91a4122"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>